<commit_message>
Updated scrum file with facebook login done.
</commit_message>
<xml_diff>
--- a/scrum/scrum_sporticide.xlsx
+++ b/scrum/scrum_sporticide.xlsx
@@ -408,9 +408,8 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF595959"/>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -468,7 +467,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -505,10 +504,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -535,7 +530,7 @@
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF4F81BD"/>
+      <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FFC0504D"/>
       <rgbColor rgb="FFFFFFCC"/>
@@ -566,7 +561,7 @@
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF595959"/>
+      <rgbColor rgb="FF4F81BD"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF10243E"/>
       <rgbColor rgb="FF339966"/>
@@ -614,6 +609,15 @@
               <a:round/>
             </a:ln>
           </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
           <c:dLbls>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
@@ -706,6 +710,15 @@
               <a:round/>
             </a:ln>
           </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
           <c:dLbls>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
@@ -798,6 +811,15 @@
               <a:round/>
             </a:ln>
           </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
           <c:dLbls>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
@@ -890,6 +912,28 @@
           </c:marker>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="99ccff"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:hiLowLines>
           <c:spPr>
             <a:ln>
@@ -903,11 +947,11 @@
           <c:downBars/>
         </c:upDownBars>
         <c:marker val="1"/>
-        <c:axId val="58042542"/>
-        <c:axId val="87830512"/>
+        <c:axId val="53981398"/>
+        <c:axId val="39962110"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="58042542"/>
+        <c:axId val="53981398"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -924,14 +968,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="87830512"/>
+        <c:crossAx val="39962110"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87830512"/>
+        <c:axId val="39962110"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -955,7 +999,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="58042542"/>
+        <c:crossAx val="53981398"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:dTable>
@@ -1001,15 +1045,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>360360</xdr:colOff>
+      <xdr:colOff>387360</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>19440</xdr:rowOff>
+      <xdr:rowOff>10440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>122040</xdr:colOff>
+      <xdr:colOff>148680</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>174240</xdr:rowOff>
+      <xdr:rowOff>164880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1017,8 +1061,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8209440" y="538560"/>
-        <a:ext cx="6060960" cy="2724120"/>
+        <a:off x="8236440" y="529560"/>
+        <a:ext cx="6060600" cy="2723760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1838,8 +1882,8 @@
   </sheetPr>
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -2062,11 +2106,14 @@
       <c r="I6" s="0" t="n">
         <v>8</v>
       </c>
+      <c r="J6" s="0" t="n">
+        <v>12</v>
+      </c>
       <c r="K6" s="0" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2186,7 +2233,7 @@
       <c r="B2" s="8" t="n">
         <v>42283</v>
       </c>
-      <c r="C2" s="9" t="n">
+      <c r="C2" s="0" t="n">
         <v>29</v>
       </c>
       <c r="D2" s="0" t="n">
@@ -2203,7 +2250,7 @@
       <c r="B3" s="8" t="n">
         <v>42284</v>
       </c>
-      <c r="C3" s="9" t="n">
+      <c r="C3" s="0" t="n">
         <f aca="false">C2 - 29/15</f>
         <v>27.0666666666667</v>
       </c>
@@ -2221,7 +2268,7 @@
       <c r="B4" s="8" t="n">
         <v>42285</v>
       </c>
-      <c r="C4" s="9" t="n">
+      <c r="C4" s="0" t="n">
         <f aca="false">C3 - 29/15</f>
         <v>25.1333333333333</v>
       </c>
@@ -2239,7 +2286,7 @@
       <c r="B5" s="8" t="n">
         <v>42286</v>
       </c>
-      <c r="C5" s="9" t="n">
+      <c r="C5" s="0" t="n">
         <f aca="false">C4 - 29/15</f>
         <v>23.2</v>
       </c>
@@ -2257,7 +2304,7 @@
       <c r="B6" s="8" t="n">
         <v>42287</v>
       </c>
-      <c r="C6" s="9" t="n">
+      <c r="C6" s="0" t="n">
         <f aca="false">C5 - 29/15</f>
         <v>21.2666666666667</v>
       </c>
@@ -2275,7 +2322,7 @@
       <c r="B7" s="8" t="n">
         <v>42288</v>
       </c>
-      <c r="C7" s="9" t="n">
+      <c r="C7" s="0" t="n">
         <f aca="false">C6 - 29/15</f>
         <v>19.3333333333333</v>
       </c>
@@ -2293,7 +2340,7 @@
       <c r="B8" s="8" t="n">
         <v>42289</v>
       </c>
-      <c r="C8" s="9" t="n">
+      <c r="C8" s="0" t="n">
         <f aca="false">C7 - 29/15</f>
         <v>17.4</v>
       </c>
@@ -2311,7 +2358,7 @@
       <c r="B9" s="8" t="n">
         <v>42290</v>
       </c>
-      <c r="C9" s="9" t="n">
+      <c r="C9" s="0" t="n">
         <f aca="false">C8 - 29/15</f>
         <v>15.4666666666667</v>
       </c>
@@ -2329,7 +2376,7 @@
       <c r="B10" s="8" t="n">
         <v>42291</v>
       </c>
-      <c r="C10" s="9" t="n">
+      <c r="C10" s="0" t="n">
         <f aca="false">C9 - 29/15</f>
         <v>13.5333333333333</v>
       </c>
@@ -2341,7 +2388,7 @@
       <c r="B11" s="8" t="n">
         <v>42292</v>
       </c>
-      <c r="C11" s="9" t="n">
+      <c r="C11" s="0" t="n">
         <f aca="false">C10 - 29/15</f>
         <v>11.6</v>
       </c>
@@ -2353,7 +2400,7 @@
       <c r="B12" s="8" t="n">
         <v>42293</v>
       </c>
-      <c r="C12" s="9" t="n">
+      <c r="C12" s="0" t="n">
         <f aca="false">C11 - 29/15</f>
         <v>9.66666666666666</v>
       </c>
@@ -2365,7 +2412,7 @@
       <c r="B13" s="8" t="n">
         <v>42294</v>
       </c>
-      <c r="C13" s="9" t="n">
+      <c r="C13" s="0" t="n">
         <f aca="false">C12 - 29/15</f>
         <v>7.73333333333333</v>
       </c>
@@ -2377,7 +2424,7 @@
       <c r="B14" s="8" t="n">
         <v>42295</v>
       </c>
-      <c r="C14" s="9" t="n">
+      <c r="C14" s="0" t="n">
         <f aca="false">C13 - 29/15</f>
         <v>5.8</v>
       </c>
@@ -2389,7 +2436,7 @@
       <c r="B15" s="8" t="n">
         <v>42296</v>
       </c>
-      <c r="C15" s="9" t="n">
+      <c r="C15" s="0" t="n">
         <f aca="false">C14 - 29/15</f>
         <v>3.86666666666666</v>
       </c>
@@ -2401,7 +2448,7 @@
       <c r="B16" s="8" t="n">
         <v>42297</v>
       </c>
-      <c r="C16" s="9" t="n">
+      <c r="C16" s="0" t="n">
         <f aca="false">C15 - 29/15</f>
         <v>1.93333333333333</v>
       </c>

</xml_diff>